<commit_message>
endinger i farger og plassering
</commit_message>
<xml_diff>
--- a/visualiseringseksamenObjekter.xlsx
+++ b/visualiseringseksamenObjekter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/millemariehagen/Desktop/visualisering/VisualiseringEksamen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{228B8197-FAFA-BE46-9F3A-A808ECC7998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D597B1EE-5BDD-D546-A2D7-33AFA2AF6382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{1B8DC8FB-4DBE-6049-BD6B-A5EBDBFE80A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1B8DC8FB-4DBE-6049-BD6B-A5EBDBFE80A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
-  <si>
-    <t>informasjon om Yale chool of art</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>attributter:</t>
   </si>
@@ -174,13 +171,19 @@
   </si>
   <si>
     <t>facebook side</t>
+  </si>
+  <si>
+    <t>objekt:</t>
+  </si>
+  <si>
+    <t>informasjon til studenter om Yale chool of art</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -201,6 +204,15 @@
       <color rgb="FF000000"/>
       <name val="Times"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,11 +235,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,219 +557,232 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8958BBC4-111B-4840-8BA5-316644E759C7}">
   <dimension ref="F6:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="5.5" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="6" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G6" t="s">
-        <v>0</v>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>2</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
         <v>4</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>5</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="12" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
         <v>2</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>3</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" t="s">
         <v>4</v>
       </c>
-      <c r="J12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>5</v>
-      </c>
-      <c r="L12" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="13" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K14" s="3">
         <v>46844</v>
       </c>
       <c r="L14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="3">
         <v>46813</v>
       </c>
       <c r="L15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="6:12" ht="24" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="7:12" ht="24" x14ac:dyDescent="0.3">
       <c r="J21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="7:12" ht="19" x14ac:dyDescent="0.25">
       <c r="J22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="7:12" ht="19" x14ac:dyDescent="0.25">
       <c r="J23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="7:12" ht="19" x14ac:dyDescent="0.25">
       <c r="J24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="7:12" ht="19" x14ac:dyDescent="0.25">
       <c r="J25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>